<commit_message>
data_filt filters all LF signals with outlier removal and moving average
</commit_message>
<xml_diff>
--- a/Test_sheet.xlsx
+++ b/Test_sheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Thesis\MT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B13EA6-FCF5-4E35-930B-A117789DE6A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C736533A-4F8B-470C-B6D8-7A18B39FE218}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="1" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="2" r:id="rId1"/>
     <sheet name="Tests" sheetId="1" r:id="rId2"/>
+    <sheet name="Test plan different tension" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>Sheet for entering test data</t>
   </si>
@@ -152,13 +153,61 @@
   </si>
   <si>
     <t>T9</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Loose</t>
+  </si>
+  <si>
+    <t>Very Loose</t>
+  </si>
+  <si>
+    <t>Tensioned</t>
+  </si>
+  <si>
+    <t>Very Tensioned</t>
+  </si>
+  <si>
+    <t>Belt tension Motor(+-10)</t>
+  </si>
+  <si>
+    <t>Compressor</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>Measured tension</t>
+  </si>
+  <si>
+    <t>Tension after test</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>180deg</t>
+  </si>
+  <si>
+    <t>~140</t>
+  </si>
+  <si>
+    <t>~160</t>
+  </si>
+  <si>
+    <t>Tests for  T2-T10_steady_t95-t180</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +230,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -191,8 +247,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -385,10 +440,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -412,14 +468,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bra" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -735,7 +799,7 @@
   <dimension ref="A3:E26"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,111 +839,127 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="23">
+      <c r="A6" s="24">
         <v>1</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="26">
         <v>225</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="27">
         <v>800</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="28">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="24">
         <v>2</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8">
+      <c r="B7" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="24">
         <v>3</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8">
+      <c r="B8" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="25">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="24">
         <v>4</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7">
+      <c r="B9" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="24"/>
+      <c r="D9" s="29">
         <v>1300</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="25">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+      <c r="A10" s="24">
         <v>5</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8">
+      <c r="B10" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="24">
         <v>6</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8">
+      <c r="B11" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="25">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="24">
         <v>7</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7">
+      <c r="B12" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="29">
         <v>1800</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="25">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="24">
         <v>8</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8">
+      <c r="B13" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="25">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="9">
+      <c r="A14" s="30">
         <v>9</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11">
+      <c r="B14" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="31">
         <v>22</v>
       </c>
     </row>
@@ -1014,7 +1094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ADE930-95F2-4FE7-8425-1D0ED343DBA9}">
   <dimension ref="B2:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
@@ -1456,31 +1536,31 @@
       <c r="K26" s="15"/>
     </row>
     <row r="29" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28" t="s">
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28" t="s">
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28" t="s">
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28" t="s">
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="O29" s="28"/>
-      <c r="P29" s="28"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
       <c r="Q29" t="s">
         <v>39</v>
       </c>
@@ -2714,4 +2794,189 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09D7FBE0-FB77-446D-8C3D-573F9BCE60AC}">
+  <dimension ref="B1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="17">
+        <v>100</v>
+      </c>
+      <c r="E3" s="18">
+        <v>810</v>
+      </c>
+      <c r="F3" s="19">
+        <v>10</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="14">
+        <v>125</v>
+      </c>
+      <c r="J3" s="14">
+        <v>100</v>
+      </c>
+      <c r="K3" s="34"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="6">
+        <v>120</v>
+      </c>
+      <c r="E4" s="7">
+        <v>810</v>
+      </c>
+      <c r="F4" s="8">
+        <v>10</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14">
+        <f>AVERAGEA(128, 110, 127, 125, 118, 120, 123, 122, 127, 126)</f>
+        <v>122.6</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6">
+        <v>140</v>
+      </c>
+      <c r="E5" s="7">
+        <v>810</v>
+      </c>
+      <c r="F5" s="8">
+        <v>10</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6">
+        <v>160</v>
+      </c>
+      <c r="E6" s="7">
+        <v>810</v>
+      </c>
+      <c r="F6" s="8">
+        <v>10</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="33">
+        <v>180</v>
+      </c>
+      <c r="E7" s="10">
+        <v>810</v>
+      </c>
+      <c r="F7" s="11">
+        <v>10</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15">
+        <v>180</v>
+      </c>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added test to excel sheet
</commit_message>
<xml_diff>
--- a/Test_sheet.xlsx
+++ b/Test_sheet.xlsx
@@ -8,14 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Thesis\MT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C736533A-4F8B-470C-B6D8-7A18B39FE218}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B413DE0E-AAC5-48C9-A5DC-25150550637D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="2" activeTab="5" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="2" r:id="rId1"/>
-    <sheet name="Tests" sheetId="1" r:id="rId2"/>
-    <sheet name="Test plan different tension" sheetId="3" r:id="rId3"/>
+    <sheet name="Test plan 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Tests 2018-04-20" sheetId="1" r:id="rId3"/>
+    <sheet name="Tests 2018-04-24" sheetId="3" r:id="rId4"/>
+    <sheet name="Tests 2018-04-26" sheetId="5" r:id="rId5"/>
+    <sheet name="Tests 2018-04-27" sheetId="6" r:id="rId6"/>
+    <sheet name="Changes to rig and DAQ" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="118">
   <si>
     <t>Sheet for entering test data</t>
   </si>
@@ -200,7 +204,187 @@
     <t>~160</t>
   </si>
   <si>
-    <t>Tests for  T2-T10_steady_t95-t180</t>
+    <t>Tests for  T1-T12_steady/trans_t95-t180</t>
+  </si>
+  <si>
+    <t>Compressor status</t>
+  </si>
+  <si>
+    <t>On</t>
+  </si>
+  <si>
+    <t>170-180</t>
+  </si>
+  <si>
+    <t>Warm up test with compressor initally off, then turned on, 24 Ampere, 810 RPM, 170-180 tension</t>
+  </si>
+  <si>
+    <t>Test.nr</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>0-24</t>
+  </si>
+  <si>
+    <t>0-810</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>T_after</t>
+  </si>
+  <si>
+    <t>175-185</t>
+  </si>
+  <si>
+    <t>180-200</t>
+  </si>
+  <si>
+    <t>Warm up</t>
+  </si>
+  <si>
+    <t>T1_t200_i24_rpm1600</t>
+  </si>
+  <si>
+    <t>21-22</t>
+  </si>
+  <si>
+    <t>22-23</t>
+  </si>
+  <si>
+    <t>Reduced speed, same setup</t>
+  </si>
+  <si>
+    <t>RPM[840,1200,1590]</t>
+  </si>
+  <si>
+    <t>T2_t200_i24_rpm1200</t>
+  </si>
+  <si>
+    <t>T3_t200_i24_rpm800</t>
+  </si>
+  <si>
+    <t>Reduced speed, same setup, and cooldown in same test</t>
+  </si>
+  <si>
+    <t>am</t>
+  </si>
+  <si>
+    <t>pm</t>
+  </si>
+  <si>
+    <t>Heat from roof</t>
+  </si>
+  <si>
+    <t>T4_t100_i24_rpm1600</t>
+  </si>
+  <si>
+    <t>T6_t100_i24_rpm800</t>
+  </si>
+  <si>
+    <t>T5_t100_i24_rpm1200</t>
+  </si>
+  <si>
+    <t>Same as test 1 but with 100 in tension, start from cold(2 hours lunch)</t>
+  </si>
+  <si>
+    <t>from test 4, compressor off, decreasing speed to 1200, then compressor on, door opened after 7mins, 14:30 roof heat turned down</t>
+  </si>
+  <si>
+    <t>Test for high tension with compressor on, from warmed up to steady state, change current to 21 in name, long run to determine the top temperature of tensioner pulley, adjusted fan power</t>
+  </si>
+  <si>
+    <t>from test 5, compressor off, decreasing speed to 800, then compressor on, compressor off from 13:25, ramp down</t>
+  </si>
+  <si>
+    <t>T_after_comp</t>
+  </si>
+  <si>
+    <t>T_Comp</t>
+  </si>
+  <si>
+    <t>Tensioned to 200, running for 20 minutes, ramp down,stop, 2,5 turns cw</t>
+  </si>
+  <si>
+    <t>0-1500</t>
+  </si>
+  <si>
+    <t>T7_t75_i24_rpm800</t>
+  </si>
+  <si>
+    <t>hz</t>
+  </si>
+  <si>
+    <t>3 turns a-cw (100-110), 1 turn extra a-cw(80-90), another 0,5 a-cw(75), ramp up without load, fans on 4:20, comp on 4:40, door opens 11:00, changing load for a period, cooldown</t>
+  </si>
+  <si>
+    <t>78,79,70,77,80</t>
+  </si>
+  <si>
+    <t>No load</t>
+  </si>
+  <si>
+    <t>No load, same as before</t>
+  </si>
+  <si>
+    <t>T9_t75_i24_rpm1200</t>
+  </si>
+  <si>
+    <t>T12_t300_i24_rpm1200</t>
+  </si>
+  <si>
+    <t>T8_t75_i24_rpm800_noLoad</t>
+  </si>
+  <si>
+    <t>9.0-10.0</t>
+  </si>
+  <si>
+    <t>No load, same as before, ramp down lunch break</t>
+  </si>
+  <si>
+    <t>test1200Load</t>
+  </si>
+  <si>
+    <t>9.0-10</t>
+  </si>
+  <si>
+    <t>added load from 120 rpm without load, removed load, cooldown</t>
+  </si>
+  <si>
+    <t>9_2</t>
+  </si>
+  <si>
+    <t>T11_t300_i24_rpm1600</t>
+  </si>
+  <si>
+    <t>moved thermo couple on pulley</t>
+  </si>
+  <si>
+    <t>5 turns cw(230),2 turn cw(250), 1 turn cw(250), 1turn cw(), 0.5 turn a-cw(310,370), 0.5 a-cw. , ramp up then load on</t>
+  </si>
+  <si>
+    <t>T10_t75_i24_rpm1600</t>
+  </si>
+  <si>
+    <t>card board is loose, warm air enters compressor area</t>
+  </si>
+  <si>
+    <t>ramp down to 1200 from 1600, clutch off and on</t>
+  </si>
+  <si>
+    <t>T13_t300_i24_rpm800</t>
+  </si>
+  <si>
+    <t>card borad back in place</t>
+  </si>
+  <si>
+    <t>same as T12, pulley temperature strange in 03:40:00 clutch off/ on/ off, ramp down</t>
   </si>
 </sst>
 </file>
@@ -251,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -439,12 +623,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -481,6 +676,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bra" xfId="1" builtinId="26"/>
@@ -799,7 +1000,7 @@
   <dimension ref="A3:E26"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1091,10 +1292,173 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05EECE0-6CF0-4AA4-A814-E04E97D60F20}">
+  <dimension ref="B2:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" customWidth="1"/>
+    <col min="7" max="7" width="16.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="19"/>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="17">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18">
+        <v>180</v>
+      </c>
+      <c r="E5" s="18">
+        <v>810</v>
+      </c>
+      <c r="F5" s="19">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="6">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="6">
+        <v>4</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7">
+        <v>1320</v>
+      </c>
+      <c r="F8" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="6">
+        <v>5</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="6">
+        <v>6</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="6">
+        <v>7</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7">
+        <v>1800</v>
+      </c>
+      <c r="F11" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="6">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="9">
+        <v>9</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="11">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ADE930-95F2-4FE7-8425-1D0ED343DBA9}">
   <dimension ref="B2:V61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E39" workbookViewId="0">
       <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
@@ -2796,12 +3160,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09D7FBE0-FB77-446D-8C3D-573F9BCE60AC}">
-  <dimension ref="B1:K10"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2815,10 +3179,13 @@
     <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
       <c r="B2" s="12" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>13</v>
@@ -2845,7 +3212,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="17" t="s">
         <v>44</v>
       </c>
@@ -2872,7 +3239,7 @@
       </c>
       <c r="K3" s="34"/>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>43</v>
       </c>
@@ -2900,7 +3267,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>42</v>
       </c>
@@ -2925,7 +3292,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="s">
         <v>45</v>
       </c>
@@ -2946,9 +3313,11 @@
       <c r="J6" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="14"/>
-    </row>
-    <row r="7" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K6" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
         <v>46</v>
       </c>
@@ -2966,14 +3335,728 @@
         <v>49</v>
       </c>
       <c r="I7" s="15"/>
-      <c r="J7" s="15">
-        <v>180</v>
+      <c r="J7" s="15" t="s">
+        <v>60</v>
       </c>
       <c r="K7" s="15"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>57</v>
+      </c>
+      <c r="E10" s="36">
+        <v>43214</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFF44D6-F28F-416F-BD0F-FE0907501C17}">
+  <dimension ref="A3:S26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="36">
+        <v>43216</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>76</v>
+      </c>
+      <c r="S3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4">
+        <v>175</v>
+      </c>
+      <c r="O4" t="s">
+        <v>69</v>
+      </c>
+      <c r="P4" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>88</v>
+      </c>
+      <c r="N6" t="s">
+        <v>70</v>
+      </c>
+      <c r="P6" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q6">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P8" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q8">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+      <c r="N10" t="s">
+        <v>70</v>
+      </c>
+      <c r="O10">
+        <v>200</v>
+      </c>
+      <c r="P10">
+        <v>23</v>
+      </c>
+      <c r="Q10">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13">
+        <v>100</v>
+      </c>
+      <c r="P13">
+        <v>22</v>
+      </c>
+      <c r="Q13">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+      <c r="N15">
+        <v>100</v>
+      </c>
+      <c r="P15">
+        <v>23</v>
+      </c>
+      <c r="Q15">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="N17">
+        <v>100</v>
+      </c>
+      <c r="O17">
+        <v>130</v>
+      </c>
+      <c r="P17">
+        <v>23</v>
+      </c>
+      <c r="Q17">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="E26" s="39"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B0C3879-5E2A-4649-AB17-2527565AA58B}">
+  <dimension ref="B3:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B3" s="38">
+        <v>43217</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="R3" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="S3" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="T3" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="U3" s="39" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>92</v>
+      </c>
+      <c r="O4">
+        <v>200</v>
+      </c>
+      <c r="P4">
+        <v>200</v>
+      </c>
+      <c r="R4">
+        <v>220</v>
+      </c>
+      <c r="T4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="O6">
+        <v>75</v>
+      </c>
+      <c r="P6" t="s">
+        <v>97</v>
+      </c>
+      <c r="R6">
+        <v>100</v>
+      </c>
+      <c r="S6" t="s">
+        <v>73</v>
+      </c>
+      <c r="T6">
+        <v>840</v>
+      </c>
+      <c r="U6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>99</v>
+      </c>
+      <c r="O8">
+        <v>75</v>
+      </c>
+      <c r="P8">
+        <v>75</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="R8">
+        <v>100</v>
+      </c>
+      <c r="S8" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="T8">
+        <v>840</v>
+      </c>
+      <c r="U8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>104</v>
+      </c>
+      <c r="O10">
+        <v>75</v>
+      </c>
+      <c r="P10">
+        <v>75</v>
+      </c>
+      <c r="Q10">
+        <v>100</v>
+      </c>
+      <c r="R10">
+        <v>100</v>
+      </c>
+      <c r="S10">
+        <v>9</v>
+      </c>
+      <c r="T10">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>98</v>
+      </c>
+      <c r="S13" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="T13">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>107</v>
+      </c>
+      <c r="O15">
+        <v>75</v>
+      </c>
+      <c r="P15">
+        <v>75</v>
+      </c>
+      <c r="Q15">
+        <v>100</v>
+      </c>
+      <c r="R15">
+        <v>100</v>
+      </c>
+      <c r="S15">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>111</v>
+      </c>
+      <c r="O17">
+        <v>300</v>
+      </c>
+      <c r="Q17">
+        <v>360</v>
+      </c>
+      <c r="S17">
+        <v>22</v>
+      </c>
+      <c r="T17">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>114</v>
+      </c>
+      <c r="O19">
+        <v>300</v>
+      </c>
+      <c r="Q19">
+        <v>360</v>
+      </c>
+      <c r="S19">
+        <v>23</v>
+      </c>
+      <c r="T19">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>117</v>
+      </c>
+      <c r="O21">
+        <v>300</v>
+      </c>
+      <c r="P21">
+        <v>250</v>
+      </c>
+      <c r="Q21">
+        <v>360</v>
+      </c>
+      <c r="R21">
+        <v>260</v>
+      </c>
+      <c r="S21">
+        <v>23</v>
+      </c>
+      <c r="T21">
+        <v>840</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB3C77A-A86C-41CC-8808-23B3DAFB340B}">
+  <dimension ref="B5:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="36">
+        <v>43217</v>
+      </c>
+      <c r="C5" s="40">
+        <v>0.60972222222222217</v>
+      </c>
+      <c r="E5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C6" s="40">
+        <v>0.63124999999999998</v>
+      </c>
+      <c r="E6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C7" s="40">
+        <v>0.65347222222222223</v>
+      </c>
+      <c r="E7" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
script to estimate speed or frequency of belt with laser data
</commit_message>
<xml_diff>
--- a/Test_sheet.xlsx
+++ b/Test_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Thesis\MT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7BF248-D274-441A-AFD0-F537B30D402F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A16D8CE-0E61-4480-BF44-20030420507B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="5" activeTab="8" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="5" activeTab="9" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <sheet name="Test 2018-05-01" sheetId="8" r:id="rId7"/>
     <sheet name="Test2018-05-03" sheetId="9" r:id="rId8"/>
     <sheet name="Test2018-05-09" sheetId="10" r:id="rId9"/>
-    <sheet name="Changes to rig and DAQ" sheetId="7" r:id="rId10"/>
+    <sheet name="Test2018-05-15" sheetId="11" r:id="rId10"/>
+    <sheet name="Blad2" sheetId="12" r:id="rId11"/>
+    <sheet name="Changes to rig and DAQ" sheetId="7" r:id="rId12"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="296">
   <si>
     <t>Sheet for entering test data</t>
   </si>
@@ -703,6 +705,225 @@
   </si>
   <si>
     <t>up 5 turns(320), down one turn, start on 40, 20 seconds on, 10 seconds off, 4 times</t>
+  </si>
+  <si>
+    <t>T63Warmup</t>
+  </si>
+  <si>
+    <t>T64AccMotor</t>
+  </si>
+  <si>
+    <t>T65AccBeam</t>
+  </si>
+  <si>
+    <t>T62Idle</t>
+  </si>
+  <si>
+    <t>fz</t>
+  </si>
+  <si>
+    <t>58-60</t>
+  </si>
+  <si>
+    <t>260-290</t>
+  </si>
+  <si>
+    <t>idle, down 2 turns, get temperatures, changed tension during test</t>
+  </si>
+  <si>
+    <t>warmup, accelerometer on motor, cable in to condenser</t>
+  </si>
+  <si>
+    <t>ramp up in beginning, compressor of 2:40, ramp down, Test starts, testing different speeds without compressor, 3:30, ramping at 4:00, 30 seconds each 200rpm</t>
+  </si>
+  <si>
+    <t>cable up, ramp up from 800, high load, compressor on 60 at seconds, ramping up from 2 min, 60 sec each step, down at 7</t>
+  </si>
+  <si>
+    <t>T66TempCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at 7:10 outer edge suface temp(45.3), inner surface 8:20 (45.5), 9:20 axis(39), moving ring(46.3), 12:10 belt contact surface on pulley (45.5) </t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L0</t>
+  </si>
+  <si>
+    <t>high load</t>
+  </si>
+  <si>
+    <t>low load</t>
+  </si>
+  <si>
+    <t>no load</t>
+  </si>
+  <si>
+    <t>1600 rpm</t>
+  </si>
+  <si>
+    <t>800 rpm</t>
+  </si>
+  <si>
+    <t>T67StartupTensionTest</t>
+  </si>
+  <si>
+    <t>accelerometer back, cable in, up 3 turns, comp on 1 min</t>
+  </si>
+  <si>
+    <t>T68Ten1RPM1600HighLoad</t>
+  </si>
+  <si>
+    <t>T69Ten1RPM1600LowLoad</t>
+  </si>
+  <si>
+    <t>T70Ten1RPM1600NoLoad</t>
+  </si>
+  <si>
+    <t>T71Ten1RPM800HighLoad</t>
+  </si>
+  <si>
+    <t>T72Ten1RPM800LowLoad</t>
+  </si>
+  <si>
+    <t>T73Ten1RPM800NoLoad</t>
+  </si>
+  <si>
+    <t>T74Ten2RPM1600HighLoad</t>
+  </si>
+  <si>
+    <t>T76Ten2RPM1600NoLoad</t>
+  </si>
+  <si>
+    <t>T77Ten2RPM800HighLoad</t>
+  </si>
+  <si>
+    <t>T78Ten2RPM800LowLoad</t>
+  </si>
+  <si>
+    <t>T79Ten2RPM800NoLoad</t>
+  </si>
+  <si>
+    <t>T80Ten3RPM1600HighLoad</t>
+  </si>
+  <si>
+    <t>T81Ten3RPM1600LowLoad</t>
+  </si>
+  <si>
+    <t>T82Ten3RPM1600NoLoad</t>
+  </si>
+  <si>
+    <t>T83Ten3RPM800HighLoad</t>
+  </si>
+  <si>
+    <t>T84Ten3RPM800LowLoad</t>
+  </si>
+  <si>
+    <t>T85Ten3RPM800NoLoad</t>
+  </si>
+  <si>
+    <t>T86Ten4RPM1600HighLoad</t>
+  </si>
+  <si>
+    <t>T87Ten4RPM1600LowLoad</t>
+  </si>
+  <si>
+    <t>T88Ten4RPM1600NoLoad</t>
+  </si>
+  <si>
+    <t>T89Ten4RPM800HighLoad</t>
+  </si>
+  <si>
+    <t>T90Ten4RPM800LowLoad</t>
+  </si>
+  <si>
+    <t>T91Ten4RPM800NoLoad</t>
+  </si>
+  <si>
+    <t>T92Ten5RPM1600HighLoad</t>
+  </si>
+  <si>
+    <t>T93Ten5RPM1600LowLoad</t>
+  </si>
+  <si>
+    <t>T94Ten5RPM1600NoLoad</t>
+  </si>
+  <si>
+    <t>T95Ten5RPM800HighLoad</t>
+  </si>
+  <si>
+    <t>T96Ten5RPM800LowLoad</t>
+  </si>
+  <si>
+    <t>T97Ten5RPM800NoLoad</t>
+  </si>
+  <si>
+    <t>Cond fan 730RPM, long test for temperature convergence, something around 1hz on belt frequency, 53hz VFD</t>
+  </si>
+  <si>
+    <t>15 seconds from last test, down to low load</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15 sec from last, pulley temp increases but only due to less air flow </t>
+  </si>
+  <si>
+    <t>810, comp on at 25 sec, stable pressure at 8, running until 10</t>
+  </si>
+  <si>
+    <t>15 from previous test, SS pressure at 6, running until 8</t>
+  </si>
+  <si>
+    <t>15 from previous, from 2 to 4</t>
+  </si>
+  <si>
+    <t>T75Ten2RPM1600LowLoad</t>
+  </si>
+  <si>
+    <t>2 turns down, pressure SS from 6 to 8</t>
+  </si>
+  <si>
+    <t>15 from previous, pressure SS from3 to 5 , 1546 RPM cond fan</t>
+  </si>
+  <si>
+    <t>15 from prev from 2 to 4</t>
+  </si>
+  <si>
+    <t>15 from previous, new rpm at 30 and comp on, SS pressure at 5 to 7</t>
+  </si>
+  <si>
+    <t>15 from previous, SS pressure 4 to 6</t>
+  </si>
+  <si>
+    <t>15 from prev. 2-4</t>
+  </si>
+  <si>
+    <t>down 4 turns,ramp up, comp on at 32, fan speed same, SS from 9 to 11</t>
+  </si>
+  <si>
+    <t>down at 15, SS pressure from 4 to 6</t>
+  </si>
+  <si>
+    <t>15 from prev, comp off after 17, from 2 to 4</t>
+  </si>
+  <si>
+    <t>ramp down 13, comp on 30, SS from 5:30 to 7:30</t>
+  </si>
+  <si>
+    <t>21 from previous, SS from 2 to 4</t>
+  </si>
+  <si>
+    <t>T86AccMotorNoBelt</t>
+  </si>
+  <si>
+    <t>15 turns up, Various speed with motor disconnected from compressor and pulley system, start from 2 min, motor RPM, Accelerometer okey</t>
   </si>
 </sst>
 </file>
@@ -1611,6 +1832,828 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C0EA6F-BF46-4DB1-8DA7-8C5497715456}">
+  <dimension ref="A1:S37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.21875" customWidth="1"/>
+    <col min="13" max="13" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39" t="s">
+        <v>227</v>
+      </c>
+      <c r="M1" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="39" t="s">
+        <v>227</v>
+      </c>
+      <c r="P1" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q1" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="R1" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="S1" s="39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>228</v>
+      </c>
+      <c r="M2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>230</v>
+      </c>
+      <c r="L3">
+        <v>50</v>
+      </c>
+      <c r="M3">
+        <v>200</v>
+      </c>
+      <c r="O3">
+        <v>79</v>
+      </c>
+      <c r="P3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>232</v>
+      </c>
+      <c r="L5">
+        <v>54</v>
+      </c>
+      <c r="M5">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>245</v>
+      </c>
+      <c r="B9">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>246</v>
+      </c>
+      <c r="M9">
+        <v>310</v>
+      </c>
+      <c r="P9">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B11">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>276</v>
+      </c>
+      <c r="M11">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>248</v>
+      </c>
+      <c r="B12">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>249</v>
+      </c>
+      <c r="B13">
+        <v>70</v>
+      </c>
+      <c r="C13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>250</v>
+      </c>
+      <c r="B15">
+        <v>71</v>
+      </c>
+      <c r="C15" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>251</v>
+      </c>
+      <c r="B16">
+        <v>72</v>
+      </c>
+      <c r="C16" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
+        <v>281</v>
+      </c>
+      <c r="N17">
+        <v>260</v>
+      </c>
+      <c r="O17">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>253</v>
+      </c>
+      <c r="B20">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
+        <v>283</v>
+      </c>
+      <c r="L20">
+        <v>48</v>
+      </c>
+      <c r="M20">
+        <v>180</v>
+      </c>
+      <c r="P20">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>282</v>
+      </c>
+      <c r="B21">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>254</v>
+      </c>
+      <c r="B22">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>255</v>
+      </c>
+      <c r="B24">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>256</v>
+      </c>
+      <c r="B25">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>257</v>
+      </c>
+      <c r="B26">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <v>198</v>
+      </c>
+      <c r="O27">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>258</v>
+      </c>
+      <c r="B29">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>289</v>
+      </c>
+      <c r="M29">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>259</v>
+      </c>
+      <c r="B30">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>260</v>
+      </c>
+      <c r="B31">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>261</v>
+      </c>
+      <c r="B33">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>262</v>
+      </c>
+      <c r="B34">
+        <v>84</v>
+      </c>
+      <c r="C34" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>263</v>
+      </c>
+      <c r="B35">
+        <v>85</v>
+      </c>
+      <c r="C35" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>294</v>
+      </c>
+      <c r="B37">
+        <v>86</v>
+      </c>
+      <c r="C37" t="s">
+        <v>295</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E939A97-44AF-4685-A249-2413A9AEB269}">
+  <dimension ref="A1:T34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1">
+        <v>1600</v>
+      </c>
+      <c r="C1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B2">
+        <v>1600</v>
+      </c>
+      <c r="C2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3">
+        <v>1600</v>
+      </c>
+      <c r="C3" t="s">
+        <v>239</v>
+      </c>
+      <c r="G3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3">
+        <f>300</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4">
+        <v>800</v>
+      </c>
+      <c r="C4" t="s">
+        <v>236</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4">
+        <f>30</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5">
+        <v>800</v>
+      </c>
+      <c r="C5" t="s">
+        <v>238</v>
+      </c>
+      <c r="G5" t="s">
+        <v>236</v>
+      </c>
+      <c r="H5" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6">
+        <v>800</v>
+      </c>
+      <c r="C6" t="s">
+        <v>239</v>
+      </c>
+      <c r="G6" t="s">
+        <v>238</v>
+      </c>
+      <c r="H6" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>239</v>
+      </c>
+      <c r="H7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>1600</v>
+      </c>
+      <c r="C8" t="s">
+        <v>236</v>
+      </c>
+      <c r="G8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>1600</v>
+      </c>
+      <c r="C9" t="s">
+        <v>238</v>
+      </c>
+      <c r="G9" t="s">
+        <v>244</v>
+      </c>
+      <c r="T9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>1600</v>
+      </c>
+      <c r="C10" t="s">
+        <v>239</v>
+      </c>
+      <c r="T10" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>800</v>
+      </c>
+      <c r="C11" t="s">
+        <v>236</v>
+      </c>
+      <c r="T11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
+        <v>800</v>
+      </c>
+      <c r="C12" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
+        <v>800</v>
+      </c>
+      <c r="C13" t="s">
+        <v>239</v>
+      </c>
+      <c r="T13" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>237</v>
+      </c>
+      <c r="B15">
+        <v>1600</v>
+      </c>
+      <c r="C15" t="s">
+        <v>236</v>
+      </c>
+      <c r="T15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>237</v>
+      </c>
+      <c r="B16">
+        <v>1600</v>
+      </c>
+      <c r="C16" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B17">
+        <v>1600</v>
+      </c>
+      <c r="C17" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18">
+        <v>800</v>
+      </c>
+      <c r="C18" t="s">
+        <v>236</v>
+      </c>
+      <c r="T18" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>237</v>
+      </c>
+      <c r="B19">
+        <v>800</v>
+      </c>
+      <c r="C19" t="s">
+        <v>238</v>
+      </c>
+      <c r="T19" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>237</v>
+      </c>
+      <c r="B20">
+        <v>800</v>
+      </c>
+      <c r="C20" t="s">
+        <v>239</v>
+      </c>
+      <c r="T20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>237</v>
+      </c>
+      <c r="B22">
+        <v>1600</v>
+      </c>
+      <c r="C22" t="s">
+        <v>236</v>
+      </c>
+      <c r="T22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>237</v>
+      </c>
+      <c r="B23">
+        <v>1600</v>
+      </c>
+      <c r="C23" t="s">
+        <v>238</v>
+      </c>
+      <c r="T23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>237</v>
+      </c>
+      <c r="B24">
+        <v>1600</v>
+      </c>
+      <c r="C24" t="s">
+        <v>239</v>
+      </c>
+      <c r="T24" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>237</v>
+      </c>
+      <c r="B25">
+        <v>800</v>
+      </c>
+      <c r="C25" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>237</v>
+      </c>
+      <c r="B26">
+        <v>800</v>
+      </c>
+      <c r="C26" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>237</v>
+      </c>
+      <c r="B27">
+        <v>800</v>
+      </c>
+      <c r="C27" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>237</v>
+      </c>
+      <c r="B29">
+        <v>1600</v>
+      </c>
+      <c r="C29" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>237</v>
+      </c>
+      <c r="B30">
+        <v>1600</v>
+      </c>
+      <c r="C30" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>237</v>
+      </c>
+      <c r="B31">
+        <v>1600</v>
+      </c>
+      <c r="C31" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>237</v>
+      </c>
+      <c r="B32">
+        <v>800</v>
+      </c>
+      <c r="C32" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>237</v>
+      </c>
+      <c r="B33">
+        <v>800</v>
+      </c>
+      <c r="C33" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>237</v>
+      </c>
+      <c r="B34">
+        <v>800</v>
+      </c>
+      <c r="C34" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB3C77A-A86C-41CC-8808-23B3DAFB340B}">
   <dimension ref="B5:E8"/>
   <sheetViews>
@@ -1833,7 +2876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52ADE930-95F2-4FE7-8425-1D0ED343DBA9}">
   <dimension ref="B2:V61"/>
   <sheetViews>
-    <sheetView topLeftCell="E21" workbookViewId="0">
+    <sheetView topLeftCell="E17" workbookViewId="0">
       <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
@@ -3886,8 +4929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEFF44D6-F28F-416F-BD0F-FE0907501C17}">
   <dimension ref="A3:S26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4971,8 +6014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E6657-E81F-4447-8DBE-8CA74E72B38B}">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="Q41" sqref="Q41"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection sqref="A1:R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added script for predicting too high tension
</commit_message>
<xml_diff>
--- a/Test_sheet.xlsx
+++ b/Test_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Thesis\MT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A16D8CE-0E61-4480-BF44-20030420507B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FB07797-013F-442B-93CF-E2DB6A65E2F4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="5" activeTab="9" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="4" activeTab="9" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="2" r:id="rId1"/>
@@ -19,12 +19,14 @@
     <sheet name="Tests 2018-04-24" sheetId="3" r:id="rId4"/>
     <sheet name="Tests 2018-04-26" sheetId="5" r:id="rId5"/>
     <sheet name="Tests 2018-04-27" sheetId="6" r:id="rId6"/>
-    <sheet name="Test 2018-05-01" sheetId="8" r:id="rId7"/>
-    <sheet name="Test2018-05-03" sheetId="9" r:id="rId8"/>
-    <sheet name="Test2018-05-09" sheetId="10" r:id="rId9"/>
-    <sheet name="Test2018-05-15" sheetId="11" r:id="rId10"/>
-    <sheet name="Blad2" sheetId="12" r:id="rId11"/>
-    <sheet name="Changes to rig and DAQ" sheetId="7" r:id="rId12"/>
+    <sheet name="Blad3" sheetId="14" r:id="rId7"/>
+    <sheet name="Test 2018-05-01" sheetId="8" r:id="rId8"/>
+    <sheet name="Test2018-05-03" sheetId="9" r:id="rId9"/>
+    <sheet name="Test2018-05-09" sheetId="10" r:id="rId10"/>
+    <sheet name="Test2018-05-15" sheetId="11" r:id="rId11"/>
+    <sheet name="Blad1" sheetId="13" r:id="rId12"/>
+    <sheet name="Blad2" sheetId="12" r:id="rId13"/>
+    <sheet name="Changes to rig and DAQ" sheetId="7" r:id="rId14"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="333">
   <si>
     <t>Sheet for entering test data</t>
   </si>
@@ -923,7 +925,118 @@
     <t>T86AccMotorNoBelt</t>
   </si>
   <si>
-    <t>15 turns up, Various speed with motor disconnected from compressor and pulley system, start from 2 min, motor RPM, Accelerometer okey</t>
+    <t>15 turns up, Various speed with motor disconnected from compressor and pulley system, start from 2 min, motor RPM, Accelerometer okey, cable in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laser </t>
+  </si>
+  <si>
+    <t>1200 rpm</t>
+  </si>
+  <si>
+    <t>12.3</t>
+  </si>
+  <si>
+    <t>8.32</t>
+  </si>
+  <si>
+    <t>16.35</t>
+  </si>
+  <si>
+    <t>Accz</t>
+  </si>
+  <si>
+    <t>40.4</t>
+  </si>
+  <si>
+    <t>59.9</t>
+  </si>
+  <si>
+    <t>79.4</t>
+  </si>
+  <si>
+    <t>storlek</t>
+  </si>
+  <si>
+    <t>0.015</t>
+  </si>
+  <si>
+    <t>0.05-0.15</t>
+  </si>
+  <si>
+    <t>första multiplen av remmen</t>
+  </si>
+  <si>
+    <t>3e multiplen av hastigheten, med rem</t>
+  </si>
+  <si>
+    <t>Utan rem inget bidrag,  bra balanserad</t>
+  </si>
+  <si>
+    <t>T74</t>
+  </si>
+  <si>
+    <t>40.34</t>
+  </si>
+  <si>
+    <t>T79</t>
+  </si>
+  <si>
+    <t>40.39</t>
+  </si>
+  <si>
+    <t>T81</t>
+  </si>
+  <si>
+    <t>78.18</t>
+  </si>
+  <si>
+    <t>T69</t>
+  </si>
+  <si>
+    <t>78.11</t>
+  </si>
+  <si>
+    <t>T68</t>
+  </si>
+  <si>
+    <t>77.73</t>
+  </si>
+  <si>
+    <t>T85</t>
+  </si>
+  <si>
+    <t>40.42</t>
+  </si>
+  <si>
+    <t>(39.67)</t>
+  </si>
+  <si>
+    <t>0.1168</t>
+  </si>
+  <si>
+    <t>0.06427</t>
+  </si>
+  <si>
+    <t>T73</t>
+  </si>
+  <si>
+    <t>40.37</t>
+  </si>
+  <si>
+    <t>39.39</t>
+  </si>
+  <si>
+    <t>0.04241</t>
+  </si>
+  <si>
+    <t>0.1023</t>
+  </si>
+  <si>
+    <t>Low tension</t>
+  </si>
+  <si>
+    <t>High tension</t>
   </si>
 </sst>
 </file>
@@ -1540,7 +1653,7 @@
   <dimension ref="A3:E26"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1832,11 +1945,558 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E6657-E81F-4447-8DBE-8CA74E72B38B}">
+  <dimension ref="A1:R44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.44140625" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="R1" s="39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>167</v>
+      </c>
+      <c r="M3">
+        <v>150</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>73</v>
+      </c>
+      <c r="R3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>170</v>
+      </c>
+      <c r="M4">
+        <v>150</v>
+      </c>
+      <c r="N4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>205</v>
+      </c>
+      <c r="M6">
+        <v>300</v>
+      </c>
+      <c r="Q6">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="M7">
+        <v>300</v>
+      </c>
+      <c r="Q7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>172</v>
+      </c>
+      <c r="M9">
+        <v>250</v>
+      </c>
+      <c r="Q9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>179</v>
+      </c>
+      <c r="B10">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>175</v>
+      </c>
+      <c r="M10">
+        <v>250</v>
+      </c>
+      <c r="Q10">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>173</v>
+      </c>
+      <c r="M12">
+        <v>220</v>
+      </c>
+      <c r="Q12">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>174</v>
+      </c>
+      <c r="M13">
+        <v>220</v>
+      </c>
+      <c r="Q13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>198</v>
+      </c>
+      <c r="M15">
+        <v>190</v>
+      </c>
+      <c r="Q15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16">
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>199</v>
+      </c>
+      <c r="M16">
+        <v>190</v>
+      </c>
+      <c r="Q16">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B18">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>200</v>
+      </c>
+      <c r="M18">
+        <v>165</v>
+      </c>
+      <c r="Q18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>185</v>
+      </c>
+      <c r="B19">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>201</v>
+      </c>
+      <c r="M19">
+        <v>165</v>
+      </c>
+      <c r="Q19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B21">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>202</v>
+      </c>
+      <c r="M21">
+        <v>140</v>
+      </c>
+      <c r="Q21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>187</v>
+      </c>
+      <c r="B22">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>203</v>
+      </c>
+      <c r="M22">
+        <v>140</v>
+      </c>
+      <c r="Q22">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>188</v>
+      </c>
+      <c r="B26">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>206</v>
+      </c>
+      <c r="M26">
+        <v>110</v>
+      </c>
+      <c r="Q26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>189</v>
+      </c>
+      <c r="B27">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>207</v>
+      </c>
+      <c r="M27">
+        <v>110</v>
+      </c>
+      <c r="Q27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>190</v>
+      </c>
+      <c r="B29">
+        <v>50</v>
+      </c>
+      <c r="C29" t="s">
+        <v>212</v>
+      </c>
+      <c r="M29">
+        <v>85</v>
+      </c>
+      <c r="Q29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
+        <v>208</v>
+      </c>
+      <c r="M30">
+        <v>85</v>
+      </c>
+      <c r="Q30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>210</v>
+      </c>
+      <c r="M32">
+        <v>70</v>
+      </c>
+      <c r="Q32">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B33">
+        <v>53</v>
+      </c>
+      <c r="C33" t="s">
+        <v>215</v>
+      </c>
+      <c r="M33">
+        <v>70</v>
+      </c>
+      <c r="Q33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>211</v>
+      </c>
+      <c r="M35">
+        <v>45</v>
+      </c>
+      <c r="Q35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>195</v>
+      </c>
+      <c r="B36">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>213</v>
+      </c>
+      <c r="M36">
+        <v>45</v>
+      </c>
+      <c r="Q36">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38">
+        <v>56</v>
+      </c>
+      <c r="C38" t="s">
+        <v>210</v>
+      </c>
+      <c r="M38" t="s">
+        <v>214</v>
+      </c>
+      <c r="O38">
+        <v>55</v>
+      </c>
+      <c r="Q38">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>197</v>
+      </c>
+      <c r="B39">
+        <v>57</v>
+      </c>
+      <c r="C39" t="s">
+        <v>215</v>
+      </c>
+      <c r="M39" t="s">
+        <v>214</v>
+      </c>
+      <c r="O39">
+        <v>55</v>
+      </c>
+      <c r="Q39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>209</v>
+      </c>
+      <c r="B41">
+        <v>58</v>
+      </c>
+      <c r="C41" t="s">
+        <v>216</v>
+      </c>
+      <c r="M41" t="s">
+        <v>214</v>
+      </c>
+      <c r="O41">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>217</v>
+      </c>
+      <c r="B42">
+        <v>59</v>
+      </c>
+      <c r="C42" t="s">
+        <v>219</v>
+      </c>
+      <c r="M42" t="s">
+        <v>214</v>
+      </c>
+      <c r="O42">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43">
+        <v>60</v>
+      </c>
+      <c r="C43" t="s">
+        <v>218</v>
+      </c>
+      <c r="M43">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>220</v>
+      </c>
+      <c r="B44">
+        <v>61</v>
+      </c>
+      <c r="C44" t="s">
+        <v>222</v>
+      </c>
+      <c r="M44">
+        <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C0EA6F-BF46-4DB1-8DA7-8C5497715456}">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2230,7 +2890,169 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345B7335-9F55-4144-89F5-D0DF162CA6B6}">
+  <dimension ref="D6:U22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="23.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>308</v>
+      </c>
+      <c r="H6" t="s">
+        <v>309</v>
+      </c>
+      <c r="L6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>296</v>
+      </c>
+      <c r="H7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="9" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>244</v>
+      </c>
+      <c r="F9" t="s">
+        <v>299</v>
+      </c>
+      <c r="H9" t="s">
+        <v>302</v>
+      </c>
+      <c r="O9" t="s">
+        <v>311</v>
+      </c>
+      <c r="P9" t="s">
+        <v>312</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>313</v>
+      </c>
+      <c r="R9" t="s">
+        <v>314</v>
+      </c>
+      <c r="S9" t="s">
+        <v>321</v>
+      </c>
+      <c r="T9" t="s">
+        <v>322</v>
+      </c>
+      <c r="U9" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>297</v>
+      </c>
+      <c r="F10" t="s">
+        <v>298</v>
+      </c>
+      <c r="H10" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="11" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" t="s">
+        <v>300</v>
+      </c>
+      <c r="H11" t="s">
+        <v>304</v>
+      </c>
+      <c r="O11" t="s">
+        <v>315</v>
+      </c>
+      <c r="P11" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>317</v>
+      </c>
+      <c r="R11" t="s">
+        <v>318</v>
+      </c>
+      <c r="S11" t="s">
+        <v>319</v>
+      </c>
+      <c r="T11" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="4:21" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>305</v>
+      </c>
+      <c r="F13" t="s">
+        <v>306</v>
+      </c>
+      <c r="H13" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="20" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>321</v>
+      </c>
+      <c r="P20" t="s">
+        <v>331</v>
+      </c>
+      <c r="R20" t="s">
+        <v>326</v>
+      </c>
+      <c r="S20" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>322</v>
+      </c>
+      <c r="P21" t="s">
+        <v>323</v>
+      </c>
+      <c r="R21" t="s">
+        <v>327</v>
+      </c>
+      <c r="S21" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="22" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O22" t="s">
+        <v>324</v>
+      </c>
+      <c r="P22" t="s">
+        <v>325</v>
+      </c>
+      <c r="R22" t="s">
+        <v>330</v>
+      </c>
+      <c r="S22" t="s">
+        <v>329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E939A97-44AF-4685-A249-2413A9AEB269}">
   <dimension ref="A1:T34"/>
   <sheetViews>
@@ -2653,7 +3475,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB3C77A-A86C-41CC-8808-23B3DAFB340B}">
   <dimension ref="B5:E8"/>
   <sheetViews>
@@ -5438,6 +6260,18 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9171600F-54C3-4629-A495-45EF1A01E741}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F287F0B2-5D14-41E7-B422-A81EE9AA7853}">
   <dimension ref="A2:T17"/>
   <sheetViews>
@@ -5716,7 +6550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A4769B-1852-45AE-9057-B8B9331FA4B4}">
   <dimension ref="A1:R18"/>
   <sheetViews>
@@ -6008,551 +6842,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E6657-E81F-4447-8DBE-8CA74E72B38B}">
-  <dimension ref="A1:R44"/>
-  <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection sqref="A1:R1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="37.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.44140625" customWidth="1"/>
-    <col min="16" max="16" width="12.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="N1" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="O1" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="P1" s="39" t="s">
-        <v>90</v>
-      </c>
-      <c r="Q1" s="39" t="s">
-        <v>134</v>
-      </c>
-      <c r="R1" s="39" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="C2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3">
-        <v>34</v>
-      </c>
-      <c r="C3" t="s">
-        <v>167</v>
-      </c>
-      <c r="M3">
-        <v>150</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>73</v>
-      </c>
-      <c r="R3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B4">
-        <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>170</v>
-      </c>
-      <c r="M4">
-        <v>150</v>
-      </c>
-      <c r="N4">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>176</v>
-      </c>
-      <c r="B6">
-        <v>36</v>
-      </c>
-      <c r="C6" t="s">
-        <v>205</v>
-      </c>
-      <c r="M6">
-        <v>300</v>
-      </c>
-      <c r="Q6">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>177</v>
-      </c>
-      <c r="B7">
-        <v>37</v>
-      </c>
-      <c r="C7" t="s">
-        <v>171</v>
-      </c>
-      <c r="M7">
-        <v>300</v>
-      </c>
-      <c r="Q7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>178</v>
-      </c>
-      <c r="B9">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>172</v>
-      </c>
-      <c r="M9">
-        <v>250</v>
-      </c>
-      <c r="Q9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>179</v>
-      </c>
-      <c r="B10">
-        <v>39</v>
-      </c>
-      <c r="C10" t="s">
-        <v>175</v>
-      </c>
-      <c r="M10">
-        <v>250</v>
-      </c>
-      <c r="Q10">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>180</v>
-      </c>
-      <c r="B12">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>173</v>
-      </c>
-      <c r="M12">
-        <v>220</v>
-      </c>
-      <c r="Q12">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>181</v>
-      </c>
-      <c r="B13">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s">
-        <v>174</v>
-      </c>
-      <c r="M13">
-        <v>220</v>
-      </c>
-      <c r="Q13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>182</v>
-      </c>
-      <c r="B15">
-        <v>42</v>
-      </c>
-      <c r="C15" t="s">
-        <v>198</v>
-      </c>
-      <c r="M15">
-        <v>190</v>
-      </c>
-      <c r="Q15">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>199</v>
-      </c>
-      <c r="M16">
-        <v>190</v>
-      </c>
-      <c r="Q16">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>184</v>
-      </c>
-      <c r="B18">
-        <v>44</v>
-      </c>
-      <c r="C18" t="s">
-        <v>200</v>
-      </c>
-      <c r="M18">
-        <v>165</v>
-      </c>
-      <c r="Q18">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>185</v>
-      </c>
-      <c r="B19">
-        <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>201</v>
-      </c>
-      <c r="M19">
-        <v>165</v>
-      </c>
-      <c r="Q19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>186</v>
-      </c>
-      <c r="B21">
-        <v>46</v>
-      </c>
-      <c r="C21" t="s">
-        <v>202</v>
-      </c>
-      <c r="M21">
-        <v>140</v>
-      </c>
-      <c r="Q21">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>187</v>
-      </c>
-      <c r="B22">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>203</v>
-      </c>
-      <c r="M22">
-        <v>140</v>
-      </c>
-      <c r="Q22">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>188</v>
-      </c>
-      <c r="B26">
-        <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>206</v>
-      </c>
-      <c r="M26">
-        <v>110</v>
-      </c>
-      <c r="Q26">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>189</v>
-      </c>
-      <c r="B27">
-        <v>49</v>
-      </c>
-      <c r="C27" t="s">
-        <v>207</v>
-      </c>
-      <c r="M27">
-        <v>110</v>
-      </c>
-      <c r="Q27">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>190</v>
-      </c>
-      <c r="B29">
-        <v>50</v>
-      </c>
-      <c r="C29" t="s">
-        <v>212</v>
-      </c>
-      <c r="M29">
-        <v>85</v>
-      </c>
-      <c r="Q29">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>191</v>
-      </c>
-      <c r="B30">
-        <v>51</v>
-      </c>
-      <c r="C30" t="s">
-        <v>208</v>
-      </c>
-      <c r="M30">
-        <v>85</v>
-      </c>
-      <c r="Q30">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>192</v>
-      </c>
-      <c r="B32">
-        <v>52</v>
-      </c>
-      <c r="C32" t="s">
-        <v>210</v>
-      </c>
-      <c r="M32">
-        <v>70</v>
-      </c>
-      <c r="Q32">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>193</v>
-      </c>
-      <c r="B33">
-        <v>53</v>
-      </c>
-      <c r="C33" t="s">
-        <v>215</v>
-      </c>
-      <c r="M33">
-        <v>70</v>
-      </c>
-      <c r="Q33">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>194</v>
-      </c>
-      <c r="B35">
-        <v>54</v>
-      </c>
-      <c r="C35" t="s">
-        <v>211</v>
-      </c>
-      <c r="M35">
-        <v>45</v>
-      </c>
-      <c r="Q35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>195</v>
-      </c>
-      <c r="B36">
-        <v>55</v>
-      </c>
-      <c r="C36" t="s">
-        <v>213</v>
-      </c>
-      <c r="M36">
-        <v>45</v>
-      </c>
-      <c r="Q36">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>196</v>
-      </c>
-      <c r="B38">
-        <v>56</v>
-      </c>
-      <c r="C38" t="s">
-        <v>210</v>
-      </c>
-      <c r="M38" t="s">
-        <v>214</v>
-      </c>
-      <c r="O38">
-        <v>55</v>
-      </c>
-      <c r="Q38">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>197</v>
-      </c>
-      <c r="B39">
-        <v>57</v>
-      </c>
-      <c r="C39" t="s">
-        <v>215</v>
-      </c>
-      <c r="M39" t="s">
-        <v>214</v>
-      </c>
-      <c r="O39">
-        <v>55</v>
-      </c>
-      <c r="Q39">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>209</v>
-      </c>
-      <c r="B41">
-        <v>58</v>
-      </c>
-      <c r="C41" t="s">
-        <v>216</v>
-      </c>
-      <c r="M41" t="s">
-        <v>214</v>
-      </c>
-      <c r="O41">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>217</v>
-      </c>
-      <c r="B42">
-        <v>59</v>
-      </c>
-      <c r="C42" t="s">
-        <v>219</v>
-      </c>
-      <c r="M42" t="s">
-        <v>214</v>
-      </c>
-      <c r="O42">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>221</v>
-      </c>
-      <c r="B43">
-        <v>60</v>
-      </c>
-      <c r="C43" t="s">
-        <v>218</v>
-      </c>
-      <c r="M43">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>220</v>
-      </c>
-      <c r="B44">
-        <v>61</v>
-      </c>
-      <c r="C44" t="s">
-        <v>222</v>
-      </c>
-      <c r="M44">
-        <v>290</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added Comp_Vec to make_data_struct and other updates
</commit_message>
<xml_diff>
--- a/Test_sheet.xlsx
+++ b/Test_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\Thesis\MT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1A8302-B027-4C81-A01E-4383A9C1F0B5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D96783-8E4C-47A6-9D12-508877B10A31}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" tabRatio="875" firstSheet="6" activeTab="16" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" tabRatio="875" firstSheet="7" activeTab="10" xr2:uid="{C499E39D-B800-4351-BD6B-5EA9E2F500E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Test plan" sheetId="2" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Blad2" sheetId="12" r:id="rId15"/>
     <sheet name="Changes to rig and DAQ" sheetId="7" r:id="rId16"/>
     <sheet name="2018-06-05" sheetId="17" r:id="rId17"/>
+    <sheet name="2018-06-08" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="439">
   <si>
     <t>Sheet for entering test data</t>
   </si>
@@ -1276,16 +1277,88 @@
     <t>Aligned  motor and tensioner pulley</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>T117_Ten180_Ramp</t>
   </si>
   <si>
     <t>T118_Ten200_810RPM</t>
   </si>
   <si>
-    <t>moved motot which increased tension</t>
-  </si>
-  <si>
     <t>retension and ramp</t>
+  </si>
+  <si>
+    <t>moved motor which increased tension</t>
+  </si>
+  <si>
+    <t>idle2</t>
+  </si>
+  <si>
+    <t>190 tension, moving belt a bit rpm&lt;90</t>
+  </si>
+  <si>
+    <t>190 tension, cool down</t>
+  </si>
+  <si>
+    <t>T119_warmup</t>
+  </si>
+  <si>
+    <t>T120_cooldown</t>
+  </si>
+  <si>
+    <t>T121</t>
+  </si>
+  <si>
+    <t>down to 0 rpm, 4 min for drive pulley to reach running temp again, increased 2 degrees, compressor 5 min to reach running temp from up 3 deg, starting again at pulleytemp 42 deg</t>
+  </si>
+  <si>
+    <t>190 tension, running 1590rpm warming up without comp. Doors opened at 17:00, temp 48.5,46,40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T121 lower tension(100), first cooldown and change of tension to 100, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">from pulley 42 up to 44.5 steady state, disturbances from change of tension, </t>
+  </si>
+  <si>
+    <t>ramp up at 09:43</t>
+  </si>
+  <si>
+    <t>T122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T122 lowest tension(75), 20 sec from previous, ramp down change tension, </t>
+  </si>
+  <si>
+    <t>at 03:22 ramp up from 42deg surface, steady state at 42.3</t>
+  </si>
+  <si>
+    <t>T123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T123 lower than lowest(50), 20 sec from previous, ramp down changed tension, </t>
+  </si>
+  <si>
+    <t>started at 03:35 from 40.5 to 40</t>
+  </si>
+  <si>
+    <t>T124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T124 Highest tension(300), 21 from previous, from steady state 39.8, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">temp in comp pulley 42.75, 38 in motor pulley, 40 ten pulley, </t>
+  </si>
+  <si>
+    <t>starting at 4:06, 35drive,38tensioner,40comp, stady state 45drive,55ten,52comp</t>
+  </si>
+  <si>
+    <t>T125</t>
+  </si>
+  <si>
+    <t>T125 same tension 1600rpm,1200 rpm at (?), 800rpm at 10:10, 0 at 30:35</t>
   </si>
 </sst>
 </file>
@@ -2197,8 +2270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B283B9B3-91D8-4E95-86EB-3E082003BD12}">
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2430,8 +2503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873E6657-E81F-4447-8DBE-8CA74E72B38B}">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2978,7 +3051,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3206,8 +3279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C0EA6F-BF46-4DB1-8DA7-8C5497715456}">
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="B14" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4247,7 +4320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4AF7FA-A6F3-4D01-AB42-2B1D537DBE0F}">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -4331,7 +4404,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B5" t="s">
         <v>414</v>
@@ -4342,13 +4415,133 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B6" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="L6">
         <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF5B19B-28DE-4B2E-AB3D-8089BD040B04}">
+  <dimension ref="A3:K17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>416</v>
+      </c>
+      <c r="C4" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>419</v>
+      </c>
+      <c r="C5" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>420</v>
+      </c>
+      <c r="C6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C7" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>427</v>
+      </c>
+      <c r="C10" t="s">
+        <v>428</v>
+      </c>
+      <c r="K10" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>430</v>
+      </c>
+      <c r="C12" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>433</v>
+      </c>
+      <c r="C14" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>437</v>
+      </c>
+      <c r="C17" t="s">
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -6785,7 +6978,7 @@
   <dimension ref="B3:U21"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>